<commit_message>
reuslt table, mailing / TW done
</commit_message>
<xml_diff>
--- a/Data/Temp/dt_finalResult.xlsx
+++ b/Data/Temp/dt_finalResult.xlsx
@@ -34,10 +34,28 @@
     <x:t>Total Due</x:t>
   </x:si>
   <x:si>
-    <x:t>su5t3u1pm99c21vf1l464r</x:t>
-  </x:si>
-  <x:si>
-    <x:t>08/28/2024 00:00:00</x:t>
+    <x:t>qggbra4vo6gg20abvansjl</x:t>
+  </x:si>
+  <x:si>
+    <x:t>07/31/2024 00:00:00</x:t>
+  </x:si>
+  <x:si>
+    <x:t>284221</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2019-06-20</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Aenean LLC</x:t>
+  </x:si>
+  <x:si>
+    <x:t>6300.00</x:t>
+  </x:si>
+  <x:si>
+    <x:t>vk8g5jf1onlhev3zli5rtl</x:t>
+  </x:si>
+  <x:si>
+    <x:t>08/19/2024 00:00:00</x:t>
   </x:si>
   <x:si>
     <x:t>284228</x:t>
@@ -46,10 +64,34 @@
     <x:t>2019-06-28</x:t>
   </x:si>
   <x:si>
-    <x:t>Aenean LLC</x:t>
-  </x:si>
-  <x:si>
     <x:t>1800.00</x:t>
+  </x:si>
+  <x:si>
+    <x:t>82bd360amnxy4i4z9jyy99</x:t>
+  </x:si>
+  <x:si>
+    <x:t>07/29/2024 00:00:00</x:t>
+  </x:si>
+  <x:si>
+    <x:t>284212</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2019-06-02</x:t>
+  </x:si>
+  <x:si>
+    <x:t>4139.60</x:t>
+  </x:si>
+  <x:si>
+    <x:t>695i7nvvpx8389pu0nsskc</x:t>
+  </x:si>
+  <x:si>
+    <x:t>284210</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2019-06-01</x:t>
+  </x:si>
+  <x:si>
+    <x:t>3000.00</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -400,7 +442,7 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:F2"/>
+  <x:dimension ref="A1:F3"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
@@ -444,6 +486,66 @@
       </x:c>
       <x:c r="F2" s="0" t="s">
         <x:v>11</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="3" spans="1:6">
+      <x:c r="A3" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="B3" s="0" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="C3" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="D3" s="0" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="E3" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="F3" s="0" t="s">
+        <x:v>16</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="4" spans="1:6">
+      <x:c r="A4" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="B4" s="0" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="C4" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="D4" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="E4" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="F4" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="5" spans="1:6">
+      <x:c r="A5" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="B5" s="0" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="C5" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="D5" s="0" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="E5" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="F5" s="0" t="s">
+        <x:v>25</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>